<commit_message>
Add coloring depending on types
</commit_message>
<xml_diff>
--- a/MakeJsons/ExpList.xlsx
+++ b/MakeJsons/ExpList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maco/Documents/Apps/Webpages/NeutrinoExperimentsOnEarth/MakeJsons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194C8B93-5BD3-A84D-B94D-E255A5973DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1EDA25-BAEB-A54F-9A96-AFABC4C8303D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="740" windowWidth="28320" windowHeight="18380" xr2:uid="{07D09D20-4562-D946-BD27-9B78457AD267}"/>
   </bookViews>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>First counts on solar neutrinos</t>
-  </si>
-  <si>
-    <t>Scintilatoin Detector</t>
   </si>
   <si>
     <t>LANSCE</t>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>Micro-Booster Neutrino Experiment</t>
+  </si>
+  <si>
+    <t>Scintillation Detector</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
   <dimension ref="A1:AI1096"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -854,19 +854,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>6</v>
@@ -875,16 +875,16 @@
         <v>7</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>8</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -932,7 +932,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -941,7 +941,7 @@
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -964,11 +964,11 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8">
         <v>28.153333</v>
@@ -981,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>26</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="5" spans="1:35">
       <c r="A5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="2">
         <v>35.867474440000002</v>
@@ -1089,21 +1089,21 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="2">
@@ -1113,7 +1113,7 @@
         <v>2019</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1136,13 +1136,13 @@
     </row>
     <row r="6" spans="1:35">
       <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1">
         <v>35.867417070000002</v>
@@ -1152,13 +1152,13 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1193,11 +1193,11 @@
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2">
         <v>36.423888900000001</v>
@@ -1206,13 +1206,13 @@
         <v>137.31972200000001</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>26</v>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="8" spans="1:35">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -1264,21 +1264,21 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="2">
@@ -1288,7 +1288,7 @@
         <v>2008</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1323,13 +1323,13 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="2">
         <v>140</v>
@@ -1345,10 +1345,10 @@
         <v>2019</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1370,13 +1370,13 @@
     </row>
     <row r="10" spans="1:35">
       <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D10" s="3">
         <v>41.834242930000002</v>
@@ -1392,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -1429,13 +1429,13 @@
     </row>
     <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2">
         <v>41.837546850000003</v>
@@ -1453,7 +1453,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1494,11 +1494,11 @@
     </row>
     <row r="12" spans="1:35">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2">
         <v>41.838606970000001</v>
@@ -1508,13 +1508,13 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1554,10 +1554,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="2">
         <v>41.8395656</v>
@@ -1612,7 +1612,7 @@
     </row>
     <row r="14" spans="1:35">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1624,21 +1624,21 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="2">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -1685,10 +1685,10 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>26</v>
@@ -1732,10 +1732,10 @@
     </row>
     <row r="16" spans="1:35">
       <c r="A16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2">
@@ -1746,10 +1746,10 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>26</v>
@@ -1766,7 +1766,7 @@
         <v>2006</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="17" spans="1:35">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1801,13 +1801,13 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1842,11 +1842,11 @@
     </row>
     <row r="18" spans="1:35">
       <c r="A18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2">
         <v>-80.800673490092095</v>
@@ -1856,19 +1856,19 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="2">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="19" spans="1:35">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1909,18 +1909,18 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="20" spans="1:35">
       <c r="A20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D20" s="2">
         <v>41.839419700000001</v>
@@ -1967,10 +1967,10 @@
         <v>-88.270137800000001</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>11</v>
@@ -1985,10 +1985,10 @@
         <v>10000</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="2">
@@ -1998,7 +1998,7 @@
         <v>2019</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>

</xml_diff>